<commit_message>
updated holidays and created csv to read in
</commit_message>
<xml_diff>
--- a/datasets/holidays.xlsx
+++ b/datasets/holidays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bicaj\Documents\Graduate Courses\DS 5220 - Supervised Machine Learning\smlproject\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9956B0A-7341-4229-BC24-825AA506FA88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E94574-5A84-431D-8CE7-B8587C965916}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{85A40F23-2F78-448B-9A40-862266829EA4}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="holidays orig" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">holidays!$A$1:$E$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">holidays!$A$1:$F$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'holidays orig'!$A$1:$E$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="133">
   <si>
     <t>Tuesday</t>
   </si>
@@ -403,6 +403,39 @@
   </si>
   <si>
     <t>Gràcia Festival</t>
+  </si>
+  <si>
+    <t>rel_city</t>
+  </si>
+  <si>
+    <t>SEVILLA</t>
+  </si>
+  <si>
+    <t>BARCELONA</t>
+  </si>
+  <si>
+    <t>Granada, Valencia, Barcelona, Sevilla</t>
+  </si>
+  <si>
+    <t>Castile-La Mancha , Valencia, Sevilla</t>
+  </si>
+  <si>
+    <t>VALENCIA</t>
+  </si>
+  <si>
+    <t>MADRID</t>
+  </si>
+  <si>
+    <t>Madrid - All</t>
+  </si>
+  <si>
+    <t>Aragon - Zaragoza is capital</t>
+  </si>
+  <si>
+    <t>PONFERRADA</t>
+  </si>
+  <si>
+    <t>Local festival</t>
   </si>
 </sst>
 </file>
@@ -798,22 +831,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD714C3E-5B86-456C-9A79-8469E1BACE5F}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.36328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="34.90625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" customWidth="1"/>
+    <col min="6" max="6" width="34.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>108</v>
       </c>
@@ -827,10 +861,13 @@
         <v>111</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43569</v>
       </c>
@@ -844,10 +881,13 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43573</v>
       </c>
@@ -860,8 +900,11 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>43574</v>
       </c>
@@ -875,10 +918,13 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>43576</v>
       </c>
@@ -892,10 +938,13 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>43577</v>
       </c>
@@ -908,8 +957,11 @@
       <c r="D6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>43578</v>
       </c>
@@ -922,11 +974,14 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>43578</v>
       </c>
@@ -940,10 +995,13 @@
         <v>36</v>
       </c>
       <c r="E8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>43578</v>
       </c>
@@ -957,10 +1015,13 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>43583</v>
       </c>
@@ -973,8 +1034,11 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>43586</v>
       </c>
@@ -988,10 +1052,13 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>43587</v>
       </c>
@@ -1005,294 +1072,814 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <v>43589</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>43590</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <v>43590</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>43591</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="7">
+        <v>43592</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="7">
+        <v>43593</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>43594</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="7">
+        <v>43594</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="7">
+        <v>43595</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="7">
+        <v>43596</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>43600</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>43590</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>43616</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>43616</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>43625</v>
+      </c>
+      <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E26" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>43594</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>43626</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>124</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>43636</v>
+      </c>
+      <c r="B28" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>43600</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>43616</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>43625</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
-        <v>43625</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <v>43626</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
-        <v>43626</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
-        <v>43636</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="C28" t="s">
         <v>62</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <v>43640</v>
-      </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <v>43692</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <v>43716</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
-        <v>43717</v>
-      </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
-        <v>43719</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
-        <v>43747</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
-        <v>43750</v>
-      </c>
-      <c r="B28" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" t="s">
-        <v>88</v>
       </c>
       <c r="D28" t="s">
         <v>2</v>
       </c>
       <c r="E28" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>43640</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>43692</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="7">
+        <v>43692</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="7">
+        <v>43693</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="7">
+        <v>43694</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="7">
+        <v>43695</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="7">
+        <v>43696</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="7">
+        <v>43697</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="7">
+        <v>43698</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>43719</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="7">
+        <v>43729</v>
+      </c>
+      <c r="B39" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="7">
+        <v>43730</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="7">
+        <v>43731</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="7">
+        <v>43732</v>
+      </c>
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="7">
+        <v>43742</v>
+      </c>
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="7">
+        <v>43743</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" t="s">
+        <v>132</v>
+      </c>
+      <c r="E44" t="s">
+        <v>124</v>
+      </c>
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="7">
+        <v>43744</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" t="s">
+        <v>132</v>
+      </c>
+      <c r="E45" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="7">
+        <v>43745</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" t="s">
+        <v>132</v>
+      </c>
+      <c r="E46" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="7">
+        <v>43746</v>
+      </c>
+      <c r="B47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" t="s">
+        <v>132</v>
+      </c>
+      <c r="E47" t="s">
+        <v>124</v>
+      </c>
+      <c r="F47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>43747</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>127</v>
+      </c>
+      <c r="F48" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="7">
+        <v>43747</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" t="s">
+        <v>124</v>
+      </c>
+      <c r="F49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="7">
+        <v>43748</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" t="s">
+        <v>132</v>
+      </c>
+      <c r="E50" t="s">
+        <v>124</v>
+      </c>
+      <c r="F50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="7">
+        <v>43749</v>
+      </c>
+      <c r="B51" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" t="s">
+        <v>132</v>
+      </c>
+      <c r="E51" t="s">
+        <v>124</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>43750</v>
+      </c>
+      <c r="B52" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="7">
+        <v>43750</v>
+      </c>
+      <c r="B53" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" t="s">
+        <v>120</v>
+      </c>
+      <c r="D53" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" t="s">
+        <v>124</v>
+      </c>
+      <c r="F53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="7">
+        <v>43751</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" t="s">
+        <v>132</v>
+      </c>
+      <c r="E54" t="s">
+        <v>124</v>
+      </c>
+      <c r="F54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
         <v>43770</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B55" t="s">
         <v>19</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C55" t="s">
         <v>89</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D55" t="s">
         <v>2</v>
       </c>
+      <c r="E55" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E29" xr:uid="{199EC6E0-E5D2-4E04-80DC-7468FFE9E7B3}"/>
+  <autoFilter ref="A1:F55" xr:uid="{199EC6E0-E5D2-4E04-80DC-7468FFE9E7B3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F55">
+    <sortCondition ref="A2:A55"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1302,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCC86F6-1A03-4C2E-870F-CACFD807CFAE}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1655,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72AD146-E37E-4D37-B50A-3096B131C434}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>